<commit_message>
finalized looking at pH check sample data to assess coefficient of variation acceptability. need to review with Karina to decide on what our cutoff would be.
</commit_message>
<xml_diff>
--- a/check sample work/pH QAQC/20201010 pH check sample results summary.xlsx
+++ b/check sample work/pH QAQC/20201010 pH check sample results summary.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="248">
   <si>
     <t>sample</t>
   </si>
@@ -768,6 +768,12 @@
   </si>
   <si>
     <t>pH at in situ</t>
+  </si>
+  <si>
+    <t>copied from below</t>
+  </si>
+  <si>
+    <t>bad sample?</t>
   </si>
 </sst>
 </file>
@@ -1977,11 +1983,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O191"/>
+  <dimension ref="A1:O192"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A196" sqref="A196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2153,6 +2159,38 @@
       <c r="E6" s="15">
         <v>7.8372515959999998</v>
       </c>
+      <c r="G6" s="15">
+        <f>AVERAGE(D6:D11)</f>
+        <v>7.9788785073333335</v>
+      </c>
+      <c r="H6" s="14">
+        <f>_xlfn.STDEV.S(D6:D11)</f>
+        <v>5.8105539598554959E-3</v>
+      </c>
+      <c r="I6" s="14">
+        <f>2*H6</f>
+        <v>1.1621107919710992E-2</v>
+      </c>
+      <c r="J6" s="14">
+        <f>H6/G6</f>
+        <v>7.2824193958023731E-4</v>
+      </c>
+      <c r="K6" s="19">
+        <f>J6</f>
+        <v>7.2824193958023731E-4</v>
+      </c>
+      <c r="L6" s="15">
+        <f>MIN(D6:D7)</f>
+        <v>7.9789145799999996</v>
+      </c>
+      <c r="M6" s="15">
+        <f>MAX(D6:D7)</f>
+        <v>7.9888786669999998</v>
+      </c>
+      <c r="N6" s="14">
+        <f>M6-L6</f>
+        <v>9.9640870000001769E-3</v>
+      </c>
     </row>
     <row r="7" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
@@ -2281,11 +2319,38 @@
       <c r="E13" s="15">
         <v>7.7897188746072503</v>
       </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="19"/>
+      <c r="G13" s="15">
+        <f>AVERAGE(D13:D15)</f>
+        <v>7.9837489199945102</v>
+      </c>
+      <c r="H13" s="14">
+        <f>_xlfn.STDEV.S(D13:D15)</f>
+        <v>6.955777388552355E-3</v>
+      </c>
+      <c r="I13" s="14">
+        <f>2*H13</f>
+        <v>1.391155477710471E-2</v>
+      </c>
+      <c r="J13" s="14">
+        <f>H13/G13</f>
+        <v>8.7124200150286515E-4</v>
+      </c>
+      <c r="K13" s="19">
+        <f>J13</f>
+        <v>8.7124200150286515E-4</v>
+      </c>
+      <c r="L13" s="15">
+        <f>MIN(D13:D14)</f>
+        <v>7.9771397199617002</v>
+      </c>
+      <c r="M13" s="15">
+        <f>MAX(D13:D14)</f>
+        <v>7.9831010909762803</v>
+      </c>
+      <c r="N13" s="14">
+        <f>M13-L13</f>
+        <v>5.9613710145800525E-3</v>
+      </c>
       <c r="O13" s="20"/>
     </row>
     <row r="14" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2348,7 +2413,7 @@
       <c r="K16" s="19"/>
       <c r="O16" s="20"/>
     </row>
-    <row r="17" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>66</v>
       </c>
@@ -2362,7 +2427,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>67</v>
       </c>
@@ -2376,7 +2441,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>68</v>
       </c>
@@ -2390,7 +2455,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>69</v>
       </c>
@@ -2404,7 +2469,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>70</v>
       </c>
@@ -2418,7 +2483,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>71</v>
       </c>
@@ -2431,8 +2496,40 @@
       <c r="E22" s="15">
         <v>7.7934605914790396</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G22" s="15">
+        <f>AVERAGE(D22:D24)</f>
+        <v>7.9574504165901736</v>
+      </c>
+      <c r="H22" s="14">
+        <f>_xlfn.STDEV.S(D22:D24)</f>
+        <v>3.248739064060405E-3</v>
+      </c>
+      <c r="I22" s="14">
+        <f>2*H22</f>
+        <v>6.4974781281208101E-3</v>
+      </c>
+      <c r="J22" s="14">
+        <f>H22/G22</f>
+        <v>4.0826381491328395E-4</v>
+      </c>
+      <c r="K22" s="19">
+        <f>J22</f>
+        <v>4.0826381491328395E-4</v>
+      </c>
+      <c r="L22" s="15">
+        <f>MIN(D22:D23)</f>
+        <v>7.9557810703072001</v>
+      </c>
+      <c r="M22" s="15">
+        <f>MAX(D22:D23)</f>
+        <v>7.9611944311944303</v>
+      </c>
+      <c r="N22" s="14">
+        <f>M22-L22</f>
+        <v>5.4133608872302119E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>72</v>
       </c>
@@ -2446,7 +2543,7 @@
         <v>7.7988739523662698</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>73</v>
       </c>
@@ -2460,7 +2557,7 @@
         <v>7.79305526944073</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>74</v>
       </c>
@@ -2473,8 +2570,40 @@
       <c r="E25" s="15">
         <v>7.9508528291040097</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="15">
+        <f>AVERAGE(D25:D27)</f>
+        <v>7.9851246943139467</v>
+      </c>
+      <c r="H25" s="14">
+        <f>_xlfn.STDEV.S(D25:D27)</f>
+        <v>4.2769810465999427E-3</v>
+      </c>
+      <c r="I25" s="14">
+        <f>2*H25</f>
+        <v>8.5539620931998853E-3</v>
+      </c>
+      <c r="J25" s="14">
+        <f>H25/G25</f>
+        <v>5.3561856706451911E-4</v>
+      </c>
+      <c r="K25" s="19">
+        <f>J25</f>
+        <v>5.3561856706451911E-4</v>
+      </c>
+      <c r="L25" s="15">
+        <f>MIN(D25:D26)</f>
+        <v>7.9812642389606001</v>
+      </c>
+      <c r="M25" s="15">
+        <f>MAX(D25:D26)</f>
+        <v>7.9843874831025499</v>
+      </c>
+      <c r="N25" s="14">
+        <f>M25-L25</f>
+        <v>3.1232441419497547E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>75</v>
       </c>
@@ -2488,7 +2617,7 @@
         <v>7.9540741754416899</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>76</v>
       </c>
@@ -2502,7 +2631,7 @@
         <v>7.9594204270895696</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>77</v>
       </c>
@@ -2516,7 +2645,7 @@
         <v>8.0873331962983404</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>78</v>
       </c>
@@ -2529,8 +2658,40 @@
       <c r="E29" s="15">
         <v>7.9828533565791204</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G29" s="15">
+        <f>AVERAGE(D29:D31)</f>
+        <v>8.1689218856547701</v>
+      </c>
+      <c r="H29" s="14">
+        <f>_xlfn.STDEV.S(D29:D31)</f>
+        <v>7.2512065917623072E-3</v>
+      </c>
+      <c r="I29" s="14">
+        <f>2*H29</f>
+        <v>1.4502413183524614E-2</v>
+      </c>
+      <c r="J29" s="14">
+        <f>H29/G29</f>
+        <v>8.8765772194442961E-4</v>
+      </c>
+      <c r="K29" s="19">
+        <f>J29</f>
+        <v>8.8765772194442961E-4</v>
+      </c>
+      <c r="L29" s="15">
+        <f>MIN(D29:D30)</f>
+        <v>8.1607421721078293</v>
+      </c>
+      <c r="M29" s="15">
+        <f>MAX(D29:D30)</f>
+        <v>8.1714628035159809</v>
+      </c>
+      <c r="N29" s="14">
+        <f>M29-L29</f>
+        <v>1.0720631408151604E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>79</v>
       </c>
@@ -2544,7 +2705,7 @@
         <v>7.9935739879872703</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>80</v>
       </c>
@@ -2558,7 +2719,7 @@
         <v>7.9966718658117797</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>81</v>
       </c>
@@ -2570,6 +2731,38 @@
       </c>
       <c r="E32" s="15">
         <v>7.8174468141535698</v>
+      </c>
+      <c r="G32" s="15">
+        <f>AVERAGE(D32:D34)</f>
+        <v>7.9602160550726255</v>
+      </c>
+      <c r="H32" s="14">
+        <f>_xlfn.STDEV.S(D32:D34)</f>
+        <v>1.1150370447331763E-2</v>
+      </c>
+      <c r="I32" s="14">
+        <f>2*H32</f>
+        <v>2.2300740894663527E-2</v>
+      </c>
+      <c r="J32" s="14">
+        <f>H32/G32</f>
+        <v>1.4007622871273979E-3</v>
+      </c>
+      <c r="K32" s="19">
+        <f>J32</f>
+        <v>1.4007622871273979E-3</v>
+      </c>
+      <c r="L32" s="15">
+        <f>MIN(D32:D33)</f>
+        <v>7.9494502463219598</v>
+      </c>
+      <c r="M32" s="15">
+        <f>MAX(D32:D33)</f>
+        <v>7.9717148226389396</v>
+      </c>
+      <c r="N32" s="14">
+        <f>M32-L32</f>
+        <v>2.2264576316979756E-2</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2613,6 +2806,38 @@
       </c>
       <c r="E35" s="15">
         <v>7.6172460390000003</v>
+      </c>
+      <c r="G35" s="15">
+        <f>AVERAGE(D35:D37)</f>
+        <v>7.7346826343333328</v>
+      </c>
+      <c r="H35" s="14">
+        <f>_xlfn.STDEV.S(D35:D37)</f>
+        <v>2.8147625800116129E-2</v>
+      </c>
+      <c r="I35" s="14">
+        <f>2*H35</f>
+        <v>5.6295251600232257E-2</v>
+      </c>
+      <c r="J35" s="14">
+        <f>H35/G35</f>
+        <v>3.6391442455792791E-3</v>
+      </c>
+      <c r="K35" s="19">
+        <f>J35</f>
+        <v>3.6391442455792791E-3</v>
+      </c>
+      <c r="L35" s="15">
+        <f>MIN(D35:D36)</f>
+        <v>7.749798792</v>
+      </c>
+      <c r="M35" s="15">
+        <f>MAX(D35:D36)</f>
+        <v>7.7520427249999999</v>
+      </c>
+      <c r="N35" s="14">
+        <f>M35-L35</f>
+        <v>2.2439329999999202E-3</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2664,6 +2889,38 @@
       <c r="E38" s="15">
         <v>7.7018438971934202</v>
       </c>
+      <c r="G38" s="15">
+        <f>AVERAGE(D38:D40)</f>
+        <v>7.8340494236955065</v>
+      </c>
+      <c r="H38" s="14">
+        <f>_xlfn.STDEV.S(D38:D40)</f>
+        <v>5.5612129855090297E-3</v>
+      </c>
+      <c r="I38" s="14">
+        <f>2*H38</f>
+        <v>1.1122425971018059E-2</v>
+      </c>
+      <c r="J38" s="14">
+        <f>H38/G38</f>
+        <v>7.098771892717616E-4</v>
+      </c>
+      <c r="K38" s="19">
+        <f>J38</f>
+        <v>7.098771892717616E-4</v>
+      </c>
+      <c r="L38" s="15">
+        <f>MIN(D38:D39)</f>
+        <v>7.83028325429615</v>
+      </c>
+      <c r="M38" s="15">
+        <f>MAX(D38:D39)</f>
+        <v>7.8404368469605803</v>
+      </c>
+      <c r="N38" s="14">
+        <f>M38-L38</f>
+        <v>1.0153592664430278E-2</v>
+      </c>
     </row>
     <row r="39" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
@@ -2706,6 +2963,38 @@
       <c r="E41" s="15">
         <v>7.6173120493425897</v>
       </c>
+      <c r="G41" s="15">
+        <f>AVERAGE(D41:D43)</f>
+        <v>7.7347934604973902</v>
+      </c>
+      <c r="H41" s="14">
+        <f>_xlfn.STDEV.S(D41:D43)</f>
+        <v>2.8061286103681849E-2</v>
+      </c>
+      <c r="I41" s="14">
+        <f>2*H41</f>
+        <v>5.6122572207363698E-2</v>
+      </c>
+      <c r="J41" s="14">
+        <f>H41/G41</f>
+        <v>3.6279295946290663E-3</v>
+      </c>
+      <c r="K41" s="19">
+        <f>J41</f>
+        <v>3.6279295946290663E-3</v>
+      </c>
+      <c r="L41" s="15">
+        <f>MIN(D41:D42)</f>
+        <v>7.7498648020787897</v>
+      </c>
+      <c r="M41" s="15">
+        <f>MAX(D41:D42)</f>
+        <v>7.7520988197778298</v>
+      </c>
+      <c r="N41" s="14">
+        <f>M41-L41</f>
+        <v>2.2340176990400806E-3</v>
+      </c>
     </row>
     <row r="42" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
@@ -2748,6 +3037,38 @@
       <c r="E44" s="15">
         <v>7.7489992873854296</v>
       </c>
+      <c r="G44" s="15">
+        <f>AVERAGE(D44:D46)</f>
+        <v>7.8425268284580163</v>
+      </c>
+      <c r="H44" s="14">
+        <f>_xlfn.STDEV.S(D44:D46)</f>
+        <v>3.4708223184882914E-3</v>
+      </c>
+      <c r="I44" s="14">
+        <f>2*H44</f>
+        <v>6.9416446369765829E-3</v>
+      </c>
+      <c r="J44" s="14">
+        <f>H44/G44</f>
+        <v>4.4256429010785012E-4</v>
+      </c>
+      <c r="K44" s="19">
+        <f>J44</f>
+        <v>4.4256429010785012E-4</v>
+      </c>
+      <c r="L44" s="15">
+        <f>MIN(D44:D45)</f>
+        <v>7.8410398633777296</v>
+      </c>
+      <c r="M44" s="15">
+        <f>MAX(D44:D45)</f>
+        <v>7.8464934009292699</v>
+      </c>
+      <c r="N44" s="14">
+        <f>M44-L44</f>
+        <v>5.4535375515403217E-3</v>
+      </c>
     </row>
     <row r="45" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
@@ -2790,6 +3111,38 @@
       <c r="E47" s="15">
         <v>7.8511536956980299</v>
       </c>
+      <c r="G47" s="15">
+        <f>AVERAGE(D47:D49)</f>
+        <v>7.9950387980165596</v>
+      </c>
+      <c r="H47" s="14">
+        <f>_xlfn.STDEV.S(D47:D49)</f>
+        <v>1.1352776695699983E-3</v>
+      </c>
+      <c r="I47" s="14">
+        <f>2*H47</f>
+        <v>2.2705553391399965E-3</v>
+      </c>
+      <c r="J47" s="14">
+        <f>H47/G47</f>
+        <v>1.4199776864768217E-4</v>
+      </c>
+      <c r="K47" s="19">
+        <f>J47</f>
+        <v>1.4199776864768217E-4</v>
+      </c>
+      <c r="L47" s="15">
+        <f>MIN(D47:D48)</f>
+        <v>7.9944032779947802</v>
+      </c>
+      <c r="M47" s="15">
+        <f>MAX(D47:D48)</f>
+        <v>7.9963495037024304</v>
+      </c>
+      <c r="N47" s="14">
+        <f>M47-L47</f>
+        <v>1.9462257076501288E-3</v>
+      </c>
     </row>
     <row r="48" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
@@ -2805,7 +3158,7 @@
         <v>7.85309992140568</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>92</v>
       </c>
@@ -2819,7 +3172,7 @@
         <v>7.8511140300557098</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>93</v>
       </c>
@@ -2833,7 +3186,7 @@
         <v>7.6858002409995496</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>94</v>
       </c>
@@ -2847,7 +3200,7 @@
         <v>7.6604061490644897</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
         <v>95</v>
       </c>
@@ -2861,7 +3214,7 @@
         <v>8.0900620266582006</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>96</v>
       </c>
@@ -2875,7 +3228,7 @@
         <v>7.6378195889536498</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>97</v>
       </c>
@@ -2889,7 +3242,7 @@
         <v>7.6496254781234603</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>98</v>
       </c>
@@ -2903,7 +3256,7 @@
         <v>8.0839369011466005</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>99</v>
       </c>
@@ -2916,8 +3269,40 @@
       <c r="E56" s="15">
         <v>7.8856255687412</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G56" s="15">
+        <f>AVERAGE(D56:D58)</f>
+        <v>8.0028052596034964</v>
+      </c>
+      <c r="H56" s="14">
+        <f>_xlfn.STDEV.S(D56:D58)</f>
+        <v>1.0911360029699298E-3</v>
+      </c>
+      <c r="I56" s="14">
+        <f>2*H56</f>
+        <v>2.1822720059398596E-3</v>
+      </c>
+      <c r="J56" s="14">
+        <f>H56/G56</f>
+        <v>1.3634419026510095E-4</v>
+      </c>
+      <c r="K56" s="19">
+        <f>J56</f>
+        <v>1.3634419026510095E-4</v>
+      </c>
+      <c r="L56" s="15">
+        <f>MIN(D56:D57)</f>
+        <v>8.0033502253286795</v>
+      </c>
+      <c r="M56" s="15">
+        <f>MAX(D56:D57)</f>
+        <v>8.0035165638346193</v>
+      </c>
+      <c r="N56" s="14">
+        <f>M56-L56</f>
+        <v>1.6633850593983368E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>100</v>
       </c>
@@ -2931,7 +3316,7 @@
         <v>7.8860289201581297</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
         <v>101</v>
       </c>
@@ -2945,7 +3330,7 @@
         <v>7.8842376073644704</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
         <v>102</v>
       </c>
@@ -2959,7 +3344,7 @@
         <v>8.0814347249955993</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
         <v>144</v>
       </c>
@@ -2972,8 +3357,12 @@
       <c r="E60" s="15">
         <v>7.1785394059999996</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G60" s="15"/>
+      <c r="K60" s="19"/>
+      <c r="L60" s="15"/>
+      <c r="M60" s="15"/>
+    </row>
+    <row r="61" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
         <v>145</v>
       </c>
@@ -2987,7 +3376,7 @@
         <v>7.1826006600000003</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
         <v>146</v>
       </c>
@@ -3001,7 +3390,7 @@
         <v>7.2032755269999997</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
         <v>131</v>
       </c>
@@ -3015,7 +3404,7 @@
         <v>7.7168752789999999</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
         <v>132</v>
       </c>
@@ -3029,7 +3418,7 @@
         <v>6.0824875330000001</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
         <v>133</v>
       </c>
@@ -3043,7 +3432,7 @@
         <v>7.7928240129999997</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
         <v>134</v>
       </c>
@@ -3057,7 +3446,7 @@
         <v>7.1200401400000004</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
         <v>135</v>
       </c>
@@ -3071,7 +3460,7 @@
         <v>7.6971565870000003</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
         <v>136</v>
       </c>
@@ -3085,7 +3474,7 @@
         <v>7.1042788000000003</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
         <v>123</v>
       </c>
@@ -3098,8 +3487,40 @@
       <c r="E69" s="15">
         <v>7.7370105999999996</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G69" s="15">
+        <f>AVERAGE(D69:D72)</f>
+        <v>7.8867945947500004</v>
+      </c>
+      <c r="H69" s="14">
+        <f>_xlfn.STDEV.S(D69:D72)</f>
+        <v>1.6129302010579652E-3</v>
+      </c>
+      <c r="I69" s="14">
+        <f>2*H69</f>
+        <v>3.2258604021159305E-3</v>
+      </c>
+      <c r="J69" s="14">
+        <f>H69/G69</f>
+        <v>2.0451023310936027E-4</v>
+      </c>
+      <c r="K69" s="19">
+        <f>J69</f>
+        <v>2.0451023310936027E-4</v>
+      </c>
+      <c r="L69" s="15">
+        <f>MIN(D69:D70)</f>
+        <v>7.8865123080000004</v>
+      </c>
+      <c r="M69" s="15">
+        <f>MAX(D69:D70)</f>
+        <v>7.8869022700000002</v>
+      </c>
+      <c r="N69" s="14">
+        <f>M69-L69</f>
+        <v>3.8996199999985492E-4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
         <v>124</v>
       </c>
@@ -3113,7 +3534,7 @@
         <v>7.7374005620000004</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
         <v>125</v>
       </c>
@@ -3127,7 +3548,7 @@
         <v>7.7393420920000002</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
         <v>126</v>
       </c>
@@ -3141,7 +3562,7 @@
         <v>7.7354182920000003</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
         <v>127</v>
       </c>
@@ -3154,8 +3575,40 @@
       <c r="E73" s="15">
         <v>7.2135083560000002</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G73" s="15">
+        <f>AVERAGE(D73:D75)</f>
+        <v>7.2621246070000005</v>
+      </c>
+      <c r="H73" s="14">
+        <f>_xlfn.STDEV.S(D73:D75)</f>
+        <v>8.9271712597115263E-2</v>
+      </c>
+      <c r="I73" s="14">
+        <f>2*H73</f>
+        <v>0.17854342519423053</v>
+      </c>
+      <c r="J73" s="14">
+        <f>H73/G73</f>
+        <v>1.2292781717221677E-2</v>
+      </c>
+      <c r="K73" s="19">
+        <f>J73</f>
+        <v>1.2292781717221677E-2</v>
+      </c>
+      <c r="L73" s="15">
+        <f>MIN(D73:D74)</f>
+        <v>7.2212618180000003</v>
+      </c>
+      <c r="M73" s="15">
+        <f>MAX(D73:D74)</f>
+        <v>7.3645139970000004</v>
+      </c>
+      <c r="N73" s="14">
+        <f>M73-L73</f>
+        <v>0.14325217900000009</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
         <v>128</v>
       </c>
@@ -3169,7 +3622,7 @@
         <v>7.0702561770000001</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
         <v>129</v>
       </c>
@@ -3183,7 +3636,7 @@
         <v>7.0495923649999996</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
         <v>130</v>
       </c>
@@ -3197,7 +3650,7 @@
         <v>8.0626476389999997</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
         <v>117</v>
       </c>
@@ -3210,8 +3663,40 @@
       <c r="E77" s="15">
         <v>7.2463720780000003</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G77" s="15">
+        <f>AVERAGE(D77:D79)</f>
+        <v>7.3893913946666672</v>
+      </c>
+      <c r="H77" s="14">
+        <f>_xlfn.STDEV.S(D77:D79)</f>
+        <v>1.0051298834871793E-2</v>
+      </c>
+      <c r="I77" s="14">
+        <f>2*H77</f>
+        <v>2.0102597669743587E-2</v>
+      </c>
+      <c r="J77" s="14">
+        <f>H77/G77</f>
+        <v>1.3602336509237246E-3</v>
+      </c>
+      <c r="K77" s="19">
+        <f>J77</f>
+        <v>1.3602336509237246E-3</v>
+      </c>
+      <c r="L77" s="15">
+        <f>MIN(D77:D78)</f>
+        <v>7.3913682520000004</v>
+      </c>
+      <c r="M77" s="15">
+        <f>MAX(D77:D78)</f>
+        <v>7.3983073910000003</v>
+      </c>
+      <c r="N77" s="14">
+        <f>M77-L77</f>
+        <v>6.9391389999999831E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
         <v>118</v>
       </c>
@@ -3225,7 +3710,7 @@
         <v>7.2533112170000003</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
         <v>119</v>
       </c>
@@ -3239,7 +3724,7 @@
         <v>7.2335023679999999</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
         <v>120</v>
       </c>
@@ -3252,8 +3737,40 @@
       <c r="E80" s="15">
         <v>7.777102953</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G80" s="15">
+        <f>AVERAGE(D80:D82)</f>
+        <v>7.9178168993333342</v>
+      </c>
+      <c r="H80" s="14">
+        <f>_xlfn.STDEV.S(D80:D82)</f>
+        <v>2.6479605817469496E-3</v>
+      </c>
+      <c r="I80" s="14">
+        <f>2*H80</f>
+        <v>5.2959211634938993E-3</v>
+      </c>
+      <c r="J80" s="14">
+        <f>H80/G80</f>
+        <v>3.344306410987987E-4</v>
+      </c>
+      <c r="K80" s="19">
+        <f>J80</f>
+        <v>3.344306410987987E-4</v>
+      </c>
+      <c r="L80" s="15">
+        <f>MIN(D80:D81)</f>
+        <v>7.9175234410000002</v>
+      </c>
+      <c r="M80" s="15">
+        <f>MAX(D80:D81)</f>
+        <v>7.9205993650000002</v>
+      </c>
+      <c r="N80" s="14">
+        <f>M80-L80</f>
+        <v>3.0759240000000077E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
         <v>121</v>
       </c>
@@ -3267,7 +3784,7 @@
         <v>7.774027029</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
         <v>122</v>
       </c>
@@ -3281,7 +3798,7 @@
         <v>7.7718314790000003</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
         <v>113</v>
       </c>
@@ -3294,8 +3811,40 @@
       <c r="E83" s="15">
         <v>7.7445232720000003</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G83" s="15">
+        <f>AVERAGE(D83:D84)</f>
+        <v>7.8792722780000002</v>
+      </c>
+      <c r="H83" s="14">
+        <f>_xlfn.STDEV.S(D83:D84)</f>
+        <v>3.9014673220513817E-3</v>
+      </c>
+      <c r="I83" s="14">
+        <f>2*H83</f>
+        <v>7.8029346441027634E-3</v>
+      </c>
+      <c r="J83" s="14">
+        <f>H83/G83</f>
+        <v>4.9515579413911216E-4</v>
+      </c>
+      <c r="K83" s="19">
+        <f>J83</f>
+        <v>4.9515579413911216E-4</v>
+      </c>
+      <c r="L83" s="15">
+        <f>MIN(D83:D84)</f>
+        <v>7.8765135239999999</v>
+      </c>
+      <c r="M83" s="15">
+        <f>MAX(D83:D84)</f>
+        <v>7.8820310320000004</v>
+      </c>
+      <c r="N83" s="14">
+        <f>M83-L83</f>
+        <v>5.5175080000005039E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
         <v>114</v>
       </c>
@@ -3309,7 +3858,7 @@
         <v>7.7390057639999998</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
         <v>115</v>
       </c>
@@ -3322,8 +3871,40 @@
       <c r="E85" s="15">
         <v>5.9870385390000003</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G85" s="15">
+        <f>AVERAGE(D85:D86)</f>
+        <v>6.324359887</v>
+      </c>
+      <c r="H85" s="14">
+        <f>_xlfn.STDEV.S(D85:D86)</f>
+        <v>0.28046397839264942</v>
+      </c>
+      <c r="I85" s="14">
+        <f>2*H85</f>
+        <v>0.56092795678529883</v>
+      </c>
+      <c r="J85" s="14">
+        <f>H85/G85</f>
+        <v>4.4346619010274139E-2</v>
+      </c>
+      <c r="K85" s="19">
+        <f>J85</f>
+        <v>4.4346619010274139E-2</v>
+      </c>
+      <c r="L85" s="15">
+        <f>MIN(D85:D86)</f>
+        <v>6.1260419060000002</v>
+      </c>
+      <c r="M85" s="15">
+        <f>MAX(D85:D86)</f>
+        <v>6.5226778679999997</v>
+      </c>
+      <c r="N85" s="14">
+        <f>M85-L85</f>
+        <v>0.39663596199999951</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
         <v>116</v>
       </c>
@@ -3337,7 +3918,7 @@
         <v>6.3836745009999998</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
         <v>137</v>
       </c>
@@ -3350,8 +3931,40 @@
       <c r="E87" s="15">
         <v>7.8171714779999997</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G87" s="15">
+        <f>AVERAGE(D87:D88)</f>
+        <v>7.9544969795</v>
+      </c>
+      <c r="H87" s="14">
+        <f>_xlfn.STDEV.S(D87:D88)</f>
+        <v>2.3728601459373456E-3</v>
+      </c>
+      <c r="I87" s="14">
+        <f>2*H87</f>
+        <v>4.7457202918746912E-3</v>
+      </c>
+      <c r="J87" s="14">
+        <f>H87/G87</f>
+        <v>2.9830423621412925E-4</v>
+      </c>
+      <c r="K87" s="19">
+        <f>J87</f>
+        <v>2.9830423621412925E-4</v>
+      </c>
+      <c r="L87" s="15">
+        <f>MIN(D87:D88)</f>
+        <v>7.9528191140000004</v>
+      </c>
+      <c r="M87" s="15">
+        <f>MAX(D87:D88)</f>
+        <v>7.9561748449999996</v>
+      </c>
+      <c r="N87" s="14">
+        <f>M87-L87</f>
+        <v>3.3557309999991958E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
         <v>138</v>
       </c>
@@ -3365,7 +3978,7 @@
         <v>7.8138157469999996</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
         <v>139</v>
       </c>
@@ -3378,8 +3991,40 @@
       <c r="E89" s="15">
         <v>7.149196559</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G89" s="15">
+        <f>AVERAGE(D89:D90)</f>
+        <v>7.3081216964999998</v>
+      </c>
+      <c r="H89" s="14">
+        <f>_xlfn.STDEV.S(D89:D90)</f>
+        <v>2.8173638027584064E-2</v>
+      </c>
+      <c r="I89" s="14">
+        <f>2*H89</f>
+        <v>5.6347276055168129E-2</v>
+      </c>
+      <c r="J89" s="14">
+        <f>H89/G89</f>
+        <v>3.8551134200566148E-3</v>
+      </c>
+      <c r="K89" s="19">
+        <f>J89</f>
+        <v>3.8551134200566148E-3</v>
+      </c>
+      <c r="L89" s="15">
+        <f>MIN(D89:D90)</f>
+        <v>7.2881999259999999</v>
+      </c>
+      <c r="M89" s="15">
+        <f>MAX(D89:D90)</f>
+        <v>7.3280434669999996</v>
+      </c>
+      <c r="N89" s="14">
+        <f>M89-L89</f>
+        <v>3.984354099999976E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
         <v>140</v>
       </c>
@@ -3393,7 +4038,7 @@
         <v>7.1890400999999997</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
         <v>141</v>
       </c>
@@ -3406,8 +4051,40 @@
       <c r="E91" s="15">
         <v>7.806159879</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G91" s="15">
+        <f>AVERAGE(D91:D93)</f>
+        <v>7.9531645400000004</v>
+      </c>
+      <c r="H91" s="14">
+        <f>_xlfn.STDEV.S(D91:D93)</f>
+        <v>5.7410776770912518E-3</v>
+      </c>
+      <c r="I91" s="14">
+        <f>2*H91</f>
+        <v>1.1482155354182504E-2</v>
+      </c>
+      <c r="J91" s="14">
+        <f>H91/G91</f>
+        <v>7.2186079493474829E-4</v>
+      </c>
+      <c r="K91" s="19">
+        <f>J91</f>
+        <v>7.2186079493474829E-4</v>
+      </c>
+      <c r="L91" s="15">
+        <f>MIN(D91:D92)</f>
+        <v>7.9557416139999999</v>
+      </c>
+      <c r="M91" s="15">
+        <f>MAX(D91:D92)</f>
+        <v>7.9571655200000002</v>
+      </c>
+      <c r="N91" s="14">
+        <f>M91-L91</f>
+        <v>1.4239060000003079E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
         <v>142</v>
       </c>
@@ -3421,7 +4098,7 @@
         <v>7.8047359729999997</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
         <v>143</v>
       </c>
@@ -3435,7 +4112,7 @@
         <v>7.7955808449999999</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
         <v>103</v>
       </c>
@@ -3448,8 +4125,40 @@
       <c r="E94" s="15">
         <v>7.803938671</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G94" s="15">
+        <f>AVERAGE(D94:D96)</f>
+        <v>7.9553642309999999</v>
+      </c>
+      <c r="H94" s="14">
+        <f>_xlfn.STDEV.S(D94:D96)</f>
+        <v>5.30163997871893E-3</v>
+      </c>
+      <c r="I94" s="14">
+        <f>2*H94</f>
+        <v>1.060327995743786E-2</v>
+      </c>
+      <c r="J94" s="14">
+        <f>H94/G94</f>
+        <v>6.6642328682573805E-4</v>
+      </c>
+      <c r="K94" s="19">
+        <f>J94</f>
+        <v>6.6642328682573805E-4</v>
+      </c>
+      <c r="L94" s="15">
+        <f>MIN(D94:D95)</f>
+        <v>7.9512931179999997</v>
+      </c>
+      <c r="M94" s="15">
+        <f>MAX(D94:D95)</f>
+        <v>7.9534403789999999</v>
+      </c>
+      <c r="N94" s="14">
+        <f>M94-L94</f>
+        <v>2.1472610000001779E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
         <v>104</v>
       </c>
@@ -3463,7 +4172,7 @@
         <v>7.8017914089999998</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
         <v>105</v>
       </c>
@@ -3477,7 +4186,7 @@
         <v>7.8118574880000002</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
         <v>106</v>
       </c>
@@ -3490,8 +4199,40 @@
       <c r="E97" s="15">
         <v>7.7740631740000001</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G97" s="15">
+        <f>AVERAGE(D97:D99)</f>
+        <v>7.9266727926666674</v>
+      </c>
+      <c r="H97" s="14">
+        <f>_xlfn.STDEV.S(D97:D99)</f>
+        <v>8.4832410898058493E-3</v>
+      </c>
+      <c r="I97" s="14">
+        <f>2*H97</f>
+        <v>1.6966482179611699E-2</v>
+      </c>
+      <c r="J97" s="14">
+        <f>H97/G97</f>
+        <v>1.0702146173680953E-3</v>
+      </c>
+      <c r="K97" s="19">
+        <f>J97</f>
+        <v>1.0702146173680953E-3</v>
+      </c>
+      <c r="L97" s="15">
+        <f>MIN(D97:D98)</f>
+        <v>7.9205601489999999</v>
+      </c>
+      <c r="M97" s="15">
+        <f>MAX(D97:D98)</f>
+        <v>7.9231002330000004</v>
+      </c>
+      <c r="N97" s="14">
+        <f>M97-L97</f>
+        <v>2.5400840000004976E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
         <v>107</v>
       </c>
@@ -3505,7 +4246,7 @@
         <v>7.7766032569999997</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
         <v>108</v>
       </c>
@@ -3519,7 +4260,7 @@
         <v>7.78986102</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="14" t="s">
         <v>109</v>
       </c>
@@ -3532,8 +4273,40 @@
       <c r="E100" s="15">
         <v>7.7964959550000001</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G100" s="15">
+        <f>AVERAGE(D100:D102)</f>
+        <v>7.9403097183333342</v>
+      </c>
+      <c r="H100" s="14">
+        <f>_xlfn.STDEV.S(D100:D102)</f>
+        <v>3.9507121649991197E-3</v>
+      </c>
+      <c r="I100" s="14">
+        <f>2*H100</f>
+        <v>7.9014243299982394E-3</v>
+      </c>
+      <c r="J100" s="14">
+        <f>H100/G100</f>
+        <v>4.9755139347742864E-4</v>
+      </c>
+      <c r="K100" s="19">
+        <f>J100</f>
+        <v>4.9755139347742864E-4</v>
+      </c>
+      <c r="L100" s="15">
+        <f>MIN(D100:D101)</f>
+        <v>7.9397894820000001</v>
+      </c>
+      <c r="M100" s="15">
+        <f>MAX(D100:D101)</f>
+        <v>7.9444947749999999</v>
+      </c>
+      <c r="N100" s="14">
+        <f>M100-L100</f>
+        <v>4.7052929999997772E-3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
         <v>110</v>
       </c>
@@ -3547,7 +4320,7 @@
         <v>7.7917906620000004</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
         <v>111</v>
       </c>
@@ -3561,7 +4334,7 @@
         <v>7.7886460780000002</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="14" t="s">
         <v>112</v>
       </c>
@@ -3574,8 +4347,12 @@
       <c r="E103" s="15">
         <v>8.1324944200000004</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G103" s="15"/>
+      <c r="K103" s="19"/>
+      <c r="L103" s="15"/>
+      <c r="M103" s="15"/>
+    </row>
+    <row r="104" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
         <v>147</v>
       </c>
@@ -3588,8 +4365,40 @@
       <c r="E104" s="15">
         <v>7.6519800279999997</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G104" s="15">
+        <f>AVERAGE(D104:D106)</f>
+        <v>7.8286223566666662</v>
+      </c>
+      <c r="H104" s="14">
+        <f>_xlfn.STDEV.S(D104:D106)</f>
+        <v>4.3084725810926235E-3</v>
+      </c>
+      <c r="I104" s="14">
+        <f>2*H104</f>
+        <v>8.616945162185247E-3</v>
+      </c>
+      <c r="J104" s="14">
+        <f>H104/G104</f>
+        <v>5.5034875675458172E-4</v>
+      </c>
+      <c r="K104" s="19">
+        <f>J104</f>
+        <v>5.5034875675458172E-4</v>
+      </c>
+      <c r="L104" s="15">
+        <f>MIN(D104:D105)</f>
+        <v>7.8241510209999996</v>
+      </c>
+      <c r="M104" s="15">
+        <f>MAX(D104:D105)</f>
+        <v>7.8327470200000002</v>
+      </c>
+      <c r="N104" s="14">
+        <f>M104-L104</f>
+        <v>8.5959990000006314E-3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
         <v>148</v>
       </c>
@@ -3603,7 +4412,7 @@
         <v>7.6605760270000003</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="14" t="s">
         <v>149</v>
       </c>
@@ -3617,7 +4426,7 @@
         <v>7.6567980359999996</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
         <v>150</v>
       </c>
@@ -3630,8 +4439,40 @@
       <c r="E107" s="15">
         <v>7.6350762339999996</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G107" s="15">
+        <f>AVERAGE(D107:D109)</f>
+        <v>7.8031815596666663</v>
+      </c>
+      <c r="H107" s="14">
+        <f>_xlfn.STDEV.S(D107:D109)</f>
+        <v>1.2324862086743652E-3</v>
+      </c>
+      <c r="I107" s="14">
+        <f>2*H107</f>
+        <v>2.4649724173487304E-3</v>
+      </c>
+      <c r="J107" s="14">
+        <f>H107/G107</f>
+        <v>1.5794662718664388E-4</v>
+      </c>
+      <c r="K107" s="19">
+        <f>J107</f>
+        <v>1.5794662718664388E-4</v>
+      </c>
+      <c r="L107" s="15">
+        <f>MIN(D107:D108)</f>
+        <v>7.8035179259999996</v>
+      </c>
+      <c r="M107" s="15">
+        <f>MAX(D107:D108)</f>
+        <v>7.8042109430000002</v>
+      </c>
+      <c r="N107" s="14">
+        <f>M107-L107</f>
+        <v>6.9301700000057309E-4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
         <v>151</v>
       </c>
@@ -3645,7 +4486,7 @@
         <v>7.6343832159999998</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="14" t="s">
         <v>152</v>
       </c>
@@ -3659,7 +4500,7 @@
         <v>7.6326811010000002</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="14" t="s">
         <v>153</v>
       </c>
@@ -3673,7 +4514,7 @@
         <v>7.6821010679999997</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="14" t="s">
         <v>154</v>
       </c>
@@ -3686,8 +4527,40 @@
       <c r="E111" s="15">
         <v>7.1358312350000004</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G111" s="15">
+        <f>AVERAGE(D111:D113)</f>
+        <v>7.3117581993333332</v>
+      </c>
+      <c r="H111" s="14">
+        <f>_xlfn.STDEV.S(D111:D113)</f>
+        <v>3.392022013306204E-3</v>
+      </c>
+      <c r="I111" s="14">
+        <f>2*H111</f>
+        <v>6.7840440266124079E-3</v>
+      </c>
+      <c r="J111" s="14">
+        <f>H111/G111</f>
+        <v>4.6391331890809512E-4</v>
+      </c>
+      <c r="K111" s="19">
+        <f>J111</f>
+        <v>4.6391331890809512E-4</v>
+      </c>
+      <c r="L111" s="15">
+        <f>MIN(D111:D112)</f>
+        <v>7.3095219609999997</v>
+      </c>
+      <c r="M111" s="15">
+        <f>MAX(D111:D112)</f>
+        <v>7.310091495</v>
+      </c>
+      <c r="N111" s="14">
+        <f>M111-L111</f>
+        <v>5.6953400000026022E-4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
         <v>155</v>
       </c>
@@ -3701,7 +4574,7 @@
         <v>7.1364007689999998</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
         <v>156</v>
       </c>
@@ -3715,7 +4588,7 @@
         <v>7.1419704160000004</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="14" t="s">
         <v>157</v>
       </c>
@@ -3728,8 +4601,40 @@
       <c r="E114" s="15">
         <v>7.4646931050000003</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G114" s="15">
+        <f>AVERAGE(D114:D116)</f>
+        <v>7.6365532553333333</v>
+      </c>
+      <c r="H114" s="14">
+        <f>_xlfn.STDEV.S(D114:D116)</f>
+        <v>2.3665927319218428E-3</v>
+      </c>
+      <c r="I114" s="14">
+        <f>2*H114</f>
+        <v>4.7331854638436857E-3</v>
+      </c>
+      <c r="J114" s="14">
+        <f>H114/G114</f>
+        <v>3.0990325776475474E-4</v>
+      </c>
+      <c r="K114" s="19">
+        <f>J114</f>
+        <v>3.0990325776475474E-4</v>
+      </c>
+      <c r="L114" s="15">
+        <f>MIN(D114:D115)</f>
+        <v>7.633827814</v>
+      </c>
+      <c r="M114" s="15">
+        <f>MAX(D114:D115)</f>
+        <v>7.6377435279999997</v>
+      </c>
+      <c r="N114" s="14">
+        <f>M114-L114</f>
+        <v>3.9157139999996815E-3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="14" t="s">
         <v>158</v>
       </c>
@@ -3743,7 +4648,7 @@
         <v>7.468608819</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="14" t="s">
         <v>159</v>
       </c>
@@ -3757,7 +4662,7 @@
         <v>7.4689537149999996</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="14" t="s">
         <v>160</v>
       </c>
@@ -3771,7 +4676,7 @@
         <v>7.6803900140000003</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="14" t="s">
         <v>161</v>
       </c>
@@ -3784,8 +4689,40 @@
       <c r="E118" s="15">
         <v>7.6667439789999996</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G118" s="15">
+        <f>AVERAGE(D118:D120)</f>
+        <v>7.8376186626666673</v>
+      </c>
+      <c r="H118" s="14">
+        <f>_xlfn.STDEV.S(D118:D120)</f>
+        <v>2.3383688385797923E-4</v>
+      </c>
+      <c r="I118" s="14">
+        <f>2*H118</f>
+        <v>4.6767376771595845E-4</v>
+      </c>
+      <c r="J118" s="14">
+        <f>H118/G118</f>
+        <v>2.9835195347258536E-5</v>
+      </c>
+      <c r="K118" s="19">
+        <f>J118</f>
+        <v>2.9835195347258536E-5</v>
+      </c>
+      <c r="L118" s="15">
+        <f>MIN(D118:D119)</f>
+        <v>7.8373963010000001</v>
+      </c>
+      <c r="M118" s="15">
+        <f>MAX(D118:D119)</f>
+        <v>7.8378624940000003</v>
+      </c>
+      <c r="N118" s="14">
+        <f>M118-L118</f>
+        <v>4.6619300000028119E-4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="14" t="s">
         <v>162</v>
       </c>
@@ -3799,7 +4736,7 @@
         <v>7.667210173</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="14" t="s">
         <v>163</v>
       </c>
@@ -3813,7 +4750,7 @@
         <v>7.6669448720000002</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="14" t="s">
         <v>164</v>
       </c>
@@ -3826,8 +4763,40 @@
       <c r="E121" s="15">
         <v>7.6503808910000002</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G121" s="15">
+        <f>AVERAGE(D121:D123)</f>
+        <v>7.8049991246666677</v>
+      </c>
+      <c r="H121" s="14">
+        <f>_xlfn.STDEV.S(D121:D123)</f>
+        <v>1.8281048603730672E-3</v>
+      </c>
+      <c r="I121" s="14">
+        <f>2*H121</f>
+        <v>3.6562097207461343E-3</v>
+      </c>
+      <c r="J121" s="14">
+        <f>H121/G121</f>
+        <v>2.3422230178035298E-4</v>
+      </c>
+      <c r="K121" s="19">
+        <f>J121</f>
+        <v>2.3422230178035298E-4</v>
+      </c>
+      <c r="L121" s="15">
+        <f>MIN(D121:D122)</f>
+        <v>7.8028915110000003</v>
+      </c>
+      <c r="M121" s="15">
+        <f>MAX(D121:D122)</f>
+        <v>7.8061551119999999</v>
+      </c>
+      <c r="N121" s="14">
+        <f>M121-L121</f>
+        <v>3.2636009999995608E-3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="14" t="s">
         <v>165</v>
       </c>
@@ -3841,7 +4810,7 @@
         <v>7.6536444919999997</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="14" t="s">
         <v>166</v>
       </c>
@@ -3855,7 +4824,7 @@
         <v>7.653440131</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="14" t="s">
         <v>167</v>
       </c>
@@ -3868,8 +4837,40 @@
       <c r="E124" s="15">
         <v>6.380766103</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G124" s="15">
+        <f>AVERAGE(D124:D126)</f>
+        <v>6.5333228156666676</v>
+      </c>
+      <c r="H124" s="14">
+        <f>_xlfn.STDEV.S(D124:D126)</f>
+        <v>5.2527046639415731E-3</v>
+      </c>
+      <c r="I124" s="14">
+        <f>2*H124</f>
+        <v>1.0505409327883146E-2</v>
+      </c>
+      <c r="J124" s="14">
+        <f>H124/G124</f>
+        <v>8.039867020416901E-4</v>
+      </c>
+      <c r="K124" s="19">
+        <f>J124</f>
+        <v>8.039867020416901E-4</v>
+      </c>
+      <c r="L124" s="15">
+        <f>MIN(D124:D125)</f>
+        <v>6.5294750800000001</v>
+      </c>
+      <c r="M124" s="15">
+        <f>MAX(D124:D125)</f>
+        <v>6.5393071149999997</v>
+      </c>
+      <c r="N124" s="14">
+        <f>M124-L124</f>
+        <v>9.8320349999996282E-3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="14" t="s">
         <v>168</v>
       </c>
@@ -3883,7 +4884,7 @@
         <v>6.3709340689999996</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="14" t="s">
         <v>169</v>
       </c>
@@ -3897,7 +4898,7 @@
         <v>6.3726452409999998</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="21" t="s">
         <v>170</v>
       </c>
@@ -3912,7 +4913,7 @@
         <v>6.9959126630000004</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="14" t="s">
         <v>171</v>
       </c>
@@ -3926,7 +4927,7 @@
         <v>7.6741815879999997</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="14" t="s">
         <v>172</v>
       </c>
@@ -3939,8 +4940,40 @@
       <c r="E129" s="15">
         <v>7.6497129179999996</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G129" s="15">
+        <f>AVERAGE(D129:D131)</f>
+        <v>7.823078547333334</v>
+      </c>
+      <c r="H129" s="14">
+        <f>_xlfn.STDEV.S(D129:D131)</f>
+        <v>1.0358335893137698E-3</v>
+      </c>
+      <c r="I129" s="14">
+        <f>2*H129</f>
+        <v>2.0716671786275395E-3</v>
+      </c>
+      <c r="J129" s="14">
+        <f>H129/G129</f>
+        <v>1.3240741263768291E-4</v>
+      </c>
+      <c r="K129" s="19">
+        <f>J129</f>
+        <v>1.3240741263768291E-4</v>
+      </c>
+      <c r="L129" s="15">
+        <f>MIN(D129:D130)</f>
+        <v>7.8218839109999996</v>
+      </c>
+      <c r="M129" s="15">
+        <f>MAX(D129:D130)</f>
+        <v>7.8236250299999996</v>
+      </c>
+      <c r="N129" s="14">
+        <f>M129-L129</f>
+        <v>1.7411190000000687E-3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="14" t="s">
         <v>173</v>
       </c>
@@ -3954,7 +4987,7 @@
         <v>7.6514540369999997</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="14" t="s">
         <v>174</v>
       </c>
@@ -3968,7 +5001,7 @@
         <v>7.6515557080000001</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="14" t="s">
         <v>175</v>
       </c>
@@ -3982,7 +5015,7 @@
         <v>7.316864421</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="14" t="s">
         <v>176</v>
       </c>
@@ -3996,7 +5029,7 @@
         <v>7.9479927589999999</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="14" t="s">
         <v>177</v>
       </c>
@@ -4010,7 +5043,7 @@
         <v>7.6949174229999997</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="14" t="s">
         <v>178</v>
       </c>
@@ -4023,8 +5056,40 @@
       <c r="E135" s="15">
         <v>7.6728612849999998</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G135" s="15">
+        <f>AVERAGE(D135:D137)</f>
+        <v>7.8371666273333327</v>
+      </c>
+      <c r="H135" s="14">
+        <f>_xlfn.STDEV.S(D135:D137)</f>
+        <v>5.7396024177454518E-3</v>
+      </c>
+      <c r="I135" s="14">
+        <f>2*H135</f>
+        <v>1.1479204835490904E-2</v>
+      </c>
+      <c r="J135" s="14">
+        <f>H135/G135</f>
+        <v>7.3235681856344606E-4</v>
+      </c>
+      <c r="K135" s="19">
+        <f>J135</f>
+        <v>7.3235681856344606E-4</v>
+      </c>
+      <c r="L135" s="15">
+        <f>MIN(D135:D136)</f>
+        <v>7.8314022960000003</v>
+      </c>
+      <c r="M135" s="15">
+        <f>MAX(D135:D136)</f>
+        <v>7.8428811769999998</v>
+      </c>
+      <c r="N135" s="14">
+        <f>M135-L135</f>
+        <v>1.1478880999999497E-2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="14" t="s">
         <v>179</v>
       </c>
@@ -4038,7 +5103,7 @@
         <v>7.6843401650000001</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="14" t="s">
         <v>180</v>
       </c>
@@ -4052,7 +5117,7 @@
         <v>7.6786753970000001</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="14" t="s">
         <v>181</v>
       </c>
@@ -4065,8 +5130,40 @@
       <c r="E138" s="15">
         <v>7.7011021179999997</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G138" s="15">
+        <f>AVERAGE(D138:D140)</f>
+        <v>7.8537295753333325</v>
+      </c>
+      <c r="H138" s="14">
+        <f>_xlfn.STDEV.S(D138:D140)</f>
+        <v>4.1681092273334356E-3</v>
+      </c>
+      <c r="I138" s="14">
+        <f>2*H138</f>
+        <v>8.3362184546668713E-3</v>
+      </c>
+      <c r="J138" s="14">
+        <f>H138/G138</f>
+        <v>5.3071718186280053E-4</v>
+      </c>
+      <c r="K138" s="19">
+        <f>J138</f>
+        <v>5.3071718186280053E-4</v>
+      </c>
+      <c r="L138" s="15">
+        <f>MIN(D138:D139)</f>
+        <v>7.8532079179999998</v>
+      </c>
+      <c r="M138" s="15">
+        <f>MAX(D138:D139)</f>
+        <v>7.8581339579999998</v>
+      </c>
+      <c r="N138" s="14">
+        <f>M138-L138</f>
+        <v>4.9260399999999649E-3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="14" t="s">
         <v>182</v>
       </c>
@@ -4080,7 +5177,7 @@
         <v>7.6961760779999997</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="14" t="s">
         <v>183</v>
       </c>
@@ -4094,7 +5191,7 @@
         <v>7.6928150100000003</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="14" t="s">
         <v>184</v>
       </c>
@@ -4107,8 +5204,40 @@
       <c r="E141" s="15">
         <v>7.6956308199999999</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G141" s="15">
+        <f>AVERAGE(D141:D143)</f>
+        <v>7.8517385473333334</v>
+      </c>
+      <c r="H141" s="14">
+        <f>_xlfn.STDEV.S(D141:D143)</f>
+        <v>6.6731049134473464E-3</v>
+      </c>
+      <c r="I141" s="14">
+        <f>2*H141</f>
+        <v>1.3346209826894693E-2</v>
+      </c>
+      <c r="J141" s="14">
+        <f>H141/G141</f>
+        <v>8.4988883330988098E-4</v>
+      </c>
+      <c r="K141" s="19">
+        <f>J141</f>
+        <v>8.4988883330988098E-4</v>
+      </c>
+      <c r="L141" s="15">
+        <f>MIN(D141:D142)</f>
+        <v>7.8466364610000001</v>
+      </c>
+      <c r="M141" s="15">
+        <f>MAX(D141:D142)</f>
+        <v>7.8492889039999998</v>
+      </c>
+      <c r="N141" s="14">
+        <f>M141-L141</f>
+        <v>2.6524429999996713E-3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="14" t="s">
         <v>185</v>
       </c>
@@ -4122,7 +5251,7 @@
         <v>7.6982832630000004</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="14" t="s">
         <v>186</v>
       </c>
@@ -4136,7 +5265,7 @@
         <v>7.7082846360000001</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="14" t="s">
         <v>187</v>
       </c>
@@ -4150,7 +5279,7 @@
         <v>7.7066703499999996</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="14" t="s">
         <v>188</v>
       </c>
@@ -4166,8 +5295,40 @@
       <c r="E145" s="15">
         <v>7.9546531288347602</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G145" s="15">
+        <f>AVERAGE(D145:D147)</f>
+        <v>8.0635118200031588</v>
+      </c>
+      <c r="H145" s="14">
+        <f>_xlfn.STDEV.S(D145:D147)</f>
+        <v>1.8254712248538549E-3</v>
+      </c>
+      <c r="I145" s="14">
+        <f>2*H145</f>
+        <v>3.6509424497077098E-3</v>
+      </c>
+      <c r="J145" s="14">
+        <f>H145/G145</f>
+        <v>2.2638662478616418E-4</v>
+      </c>
+      <c r="K145" s="19">
+        <f>J145</f>
+        <v>2.2638662478616418E-4</v>
+      </c>
+      <c r="L145" s="15">
+        <f>MIN(D145:D146)</f>
+        <v>8.0621109035941299</v>
+      </c>
+      <c r="M145" s="15">
+        <f>MAX(D145:D146)</f>
+        <v>8.0628483060290908</v>
+      </c>
+      <c r="N145" s="14">
+        <f>M145-L145</f>
+        <v>7.3740243496089874E-4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="14" t="s">
         <v>189</v>
       </c>
@@ -4184,7 +5345,7 @@
         <v>7.9539157263998002</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="14" t="s">
         <v>190</v>
       </c>
@@ -4201,7 +5362,7 @@
         <v>7.9573810731919297</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="14" t="s">
         <v>191</v>
       </c>
@@ -4217,8 +5378,40 @@
       <c r="E148" s="15">
         <v>8.0202097000015904</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G148" s="15">
+        <f>AVERAGE(D148:D150)</f>
+        <v>8.0651383830141601</v>
+      </c>
+      <c r="H148" s="14">
+        <f>_xlfn.STDEV.S(D148:D150)</f>
+        <v>3.2595699762289249E-3</v>
+      </c>
+      <c r="I148" s="14">
+        <f>2*H148</f>
+        <v>6.5191399524578498E-3</v>
+      </c>
+      <c r="J148" s="14">
+        <f>H148/G148</f>
+        <v>4.0415549261917756E-4</v>
+      </c>
+      <c r="K148" s="19">
+        <f>J148</f>
+        <v>4.0415549261917756E-4</v>
+      </c>
+      <c r="L148" s="15">
+        <f>MIN(D148:D149)</f>
+        <v>8.0629114271487694</v>
+      </c>
+      <c r="M148" s="15">
+        <f>MAX(D148:D149)</f>
+        <v>8.0688796541484091</v>
+      </c>
+      <c r="N148" s="14">
+        <f>M148-L148</f>
+        <v>5.9682269996397252E-3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="14" t="s">
         <v>192</v>
       </c>
@@ -4235,7 +5428,7 @@
         <v>8.0261779270012301</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="14" t="s">
         <v>193</v>
       </c>
@@ -4252,7 +5445,7 @@
         <v>8.0209223405981191</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="14" t="s">
         <v>194</v>
       </c>
@@ -4268,8 +5461,40 @@
       <c r="E151" s="15">
         <v>8.0323982074838405</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G151" s="15">
+        <f>AVERAGE(D151:D153)</f>
+        <v>8.1155856771348667</v>
+      </c>
+      <c r="H151" s="14">
+        <f>_xlfn.STDEV.S(D151:D153)</f>
+        <v>4.9511543134596091E-3</v>
+      </c>
+      <c r="I151" s="14">
+        <f>2*H151</f>
+        <v>9.9023086269192182E-3</v>
+      </c>
+      <c r="J151" s="14">
+        <f>H151/G151</f>
+        <v>6.1007972935448926E-4</v>
+      </c>
+      <c r="K151" s="19">
+        <f>J151</f>
+        <v>6.1007972935448926E-4</v>
+      </c>
+      <c r="L151" s="15">
+        <f>MIN(D151:D152)</f>
+        <v>8.1111947586784705</v>
+      </c>
+      <c r="M151" s="15">
+        <f>MAX(D151:D152)</f>
+        <v>8.1209519099859602</v>
+      </c>
+      <c r="N151" s="14">
+        <f>M151-L151</f>
+        <v>9.7571513074896643E-3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="14" t="s">
         <v>195</v>
       </c>
@@ -4286,7 +5511,7 @@
         <v>8.0421553587913301</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="14" t="s">
         <v>196</v>
       </c>
@@ -4303,7 +5528,7 @@
         <v>8.0358138115455393</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="14" t="s">
         <v>239</v>
       </c>
@@ -4320,7 +5545,7 @@
         <v>7.67031134315069</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="14" t="s">
         <v>197</v>
       </c>
@@ -4337,7 +5562,7 @@
         <v>8.0745769128785891</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="14" t="s">
         <v>198</v>
       </c>
@@ -4353,8 +5578,40 @@
       <c r="E156" s="15">
         <v>7.6334900193420898</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G156" s="15">
+        <f>AVERAGE(D156:D158)</f>
+        <v>7.7612406542821608</v>
+      </c>
+      <c r="H156" s="14">
+        <f>_xlfn.STDEV.S(D156:D158)</f>
+        <v>2.2324749286167411E-3</v>
+      </c>
+      <c r="I156" s="14">
+        <f>2*H156</f>
+        <v>4.4649498572334823E-3</v>
+      </c>
+      <c r="J156" s="14">
+        <f>H156/G156</f>
+        <v>2.8764408012332446E-4</v>
+      </c>
+      <c r="K156" s="19">
+        <f>J156</f>
+        <v>2.8764408012332446E-4</v>
+      </c>
+      <c r="L156" s="15">
+        <f>MIN(D156:D157)</f>
+        <v>7.7590701304939298</v>
+      </c>
+      <c r="M156" s="15">
+        <f>MAX(D156:D157)</f>
+        <v>7.7611215224821501</v>
+      </c>
+      <c r="N156" s="14">
+        <f>M156-L156</f>
+        <v>2.0513919882203524E-3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="14" t="s">
         <v>199</v>
       </c>
@@ -4371,7 +5628,7 @@
         <v>7.6355414113303102</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="14" t="s">
         <v>200</v>
       </c>
@@ -4388,7 +5645,7 @@
         <v>7.6379501987185598</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="14" t="s">
         <v>240</v>
       </c>
@@ -4405,7 +5662,7 @@
         <v>7.6830802104558602</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="14" t="s">
         <v>201</v>
       </c>
@@ -4421,8 +5678,40 @@
       <c r="E160" s="15">
         <v>7.6493613814791601</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G160" s="15">
+        <f>AVERAGE(D160:D162)</f>
+        <v>7.7712446023781139</v>
+      </c>
+      <c r="H160" s="14">
+        <f>_xlfn.STDEV.S(D160:D162)</f>
+        <v>1.4544539471623567E-3</v>
+      </c>
+      <c r="I160" s="14">
+        <f>2*H160</f>
+        <v>2.9089078943247133E-3</v>
+      </c>
+      <c r="J160" s="14">
+        <f>H160/G160</f>
+        <v>1.8715843105971373E-4</v>
+      </c>
+      <c r="K160" s="19">
+        <f>J160</f>
+        <v>1.8715843105971373E-4</v>
+      </c>
+      <c r="L160" s="15">
+        <f>MIN(D160:D161)</f>
+        <v>7.7695701272574302</v>
+      </c>
+      <c r="M160" s="15">
+        <f>MAX(D160:D161)</f>
+        <v>7.7719698752695798</v>
+      </c>
+      <c r="N160" s="14">
+        <f>M160-L160</f>
+        <v>2.399748012149594E-3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="14" t="s">
         <v>202</v>
       </c>
@@ -4439,7 +5728,7 @@
         <v>7.6469616334670096</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="14" t="s">
         <v>203</v>
       </c>
@@ -4456,7 +5745,7 @@
         <v>7.6495853108169101</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="14" t="s">
         <v>204</v>
       </c>
@@ -4476,7 +5765,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="14" t="s">
         <v>205</v>
       </c>
@@ -4496,7 +5785,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="14" t="s">
         <v>208</v>
       </c>
@@ -4509,8 +5798,40 @@
       <c r="E165" s="15">
         <v>7.8197145293565402</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G165" s="15">
+        <f>AVERAGE(D165:D166)</f>
+        <v>7.9388606092206002</v>
+      </c>
+      <c r="H165" s="14">
+        <f>_xlfn.STDEV.S(D165:D166)</f>
+        <v>2.7444127220409625E-3</v>
+      </c>
+      <c r="I165" s="14">
+        <f>2*H165</f>
+        <v>5.488825444081925E-3</v>
+      </c>
+      <c r="J165" s="14">
+        <f>H165/G165</f>
+        <v>3.456935267075304E-4</v>
+      </c>
+      <c r="K165" s="19">
+        <f>J165</f>
+        <v>3.456935267075304E-4</v>
+      </c>
+      <c r="L165" s="15">
+        <f>MIN(D165:D166)</f>
+        <v>7.9369200163744704</v>
+      </c>
+      <c r="M165" s="15">
+        <f>MAX(D165:D166)</f>
+        <v>7.94080120206673</v>
+      </c>
+      <c r="N165" s="14">
+        <f>M165-L165</f>
+        <v>3.8811856922595922E-3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="14" t="s">
         <v>209</v>
       </c>
@@ -4524,7 +5845,7 @@
         <v>7.8158333436642904</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="14" t="s">
         <v>210</v>
       </c>
@@ -4537,8 +5858,40 @@
       <c r="E167" s="15">
         <v>7.8553848262683497</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G167" s="15">
+        <f>AVERAGE(D167:D168)</f>
+        <v>7.9749337242899045</v>
+      </c>
+      <c r="H167" s="14">
+        <f>_xlfn.STDEV.S(D167:D168)</f>
+        <v>4.2441895054621441E-4</v>
+      </c>
+      <c r="I167" s="14">
+        <f>2*H167</f>
+        <v>8.4883790109242883E-4</v>
+      </c>
+      <c r="J167" s="14">
+        <f>H167/G167</f>
+        <v>5.3219119458451059E-5</v>
+      </c>
+      <c r="K167" s="19">
+        <f>J167</f>
+        <v>5.3219119458451059E-5</v>
+      </c>
+      <c r="L167" s="15">
+        <f>MIN(D167:D168)</f>
+        <v>7.9746336147719097</v>
+      </c>
+      <c r="M167" s="15">
+        <f>MAX(D167:D168)</f>
+        <v>7.9752338338079003</v>
+      </c>
+      <c r="N167" s="14">
+        <f>M167-L167</f>
+        <v>6.0021903599061233E-4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="14" t="s">
         <v>211</v>
       </c>
@@ -4552,7 +5905,7 @@
         <v>7.8559850453043403</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="14" t="s">
         <v>212</v>
       </c>
@@ -4565,8 +5918,40 @@
       <c r="E169" s="15">
         <v>7.8604470713832404</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G169" s="15">
+        <f>AVERAGE(D169:D170)</f>
+        <v>7.9873835278513656</v>
+      </c>
+      <c r="H169" s="14">
+        <f>_xlfn.STDEV.S(D169:D170)</f>
+        <v>4.8764270514582361E-4</v>
+      </c>
+      <c r="I169" s="14">
+        <f>2*H169</f>
+        <v>9.7528541029164723E-4</v>
+      </c>
+      <c r="J169" s="14">
+        <f>H169/G169</f>
+        <v>6.1051620151386578E-5</v>
+      </c>
+      <c r="K169" s="19">
+        <f>J169</f>
+        <v>6.1051620151386578E-5</v>
+      </c>
+      <c r="L169" s="15">
+        <f>MIN(D169:D170)</f>
+        <v>7.9870387123877604</v>
+      </c>
+      <c r="M169" s="15">
+        <f>MAX(D169:D170)</f>
+        <v>7.9877283433149699</v>
+      </c>
+      <c r="N169" s="14">
+        <f>M169-L169</f>
+        <v>6.8963092720952801E-4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="14" t="s">
         <v>213</v>
       </c>
@@ -4580,7 +5965,7 @@
         <v>7.8611367023104597</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="14" t="s">
         <v>214</v>
       </c>
@@ -4593,8 +5978,40 @@
       <c r="E171" s="15">
         <v>7.8679803364832699</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G171" s="15">
+        <f>AVERAGE(D171:D172)</f>
+        <v>7.9926866196154744</v>
+      </c>
+      <c r="H171" s="14">
+        <f>_xlfn.STDEV.S(D171:D172)</f>
+        <v>1.6301365956791877E-3</v>
+      </c>
+      <c r="I171" s="14">
+        <f>2*H171</f>
+        <v>3.2602731913583755E-3</v>
+      </c>
+      <c r="J171" s="14">
+        <f>H171/G171</f>
+        <v>2.0395352317186346E-4</v>
+      </c>
+      <c r="K171" s="19">
+        <f>J171</f>
+        <v>2.0395352317186346E-4</v>
+      </c>
+      <c r="L171" s="15">
+        <f>MIN(D171:D172)</f>
+        <v>7.9915339389744098</v>
+      </c>
+      <c r="M171" s="15">
+        <f>MAX(D171:D172)</f>
+        <v>7.99383930025654</v>
+      </c>
+      <c r="N171" s="14">
+        <f>M171-L171</f>
+        <v>2.3053612821302139E-3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="14" t="s">
         <v>215</v>
       </c>
@@ -4608,7 +6025,7 @@
         <v>7.8656749752011397</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="14" t="s">
         <v>225</v>
       </c>
@@ -4621,8 +6038,12 @@
       <c r="E173" s="15">
         <v>7.8735798807066004</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G173" s="15"/>
+      <c r="K173" s="19"/>
+      <c r="L173" s="15"/>
+      <c r="M173" s="15"/>
+    </row>
+    <row r="174" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="14" t="s">
         <v>216</v>
       </c>
@@ -4635,8 +6056,40 @@
       <c r="E174" s="15">
         <v>7.8674968734491202</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G174" s="15">
+        <f>AVERAGE(D174:D175)</f>
+        <v>7.9907538632896253</v>
+      </c>
+      <c r="H174" s="14">
+        <f>_xlfn.STDEV.S(D174:D175)</f>
+        <v>1.1834131828588176E-3</v>
+      </c>
+      <c r="I174" s="14">
+        <f>2*H174</f>
+        <v>2.3668263657176353E-3</v>
+      </c>
+      <c r="J174" s="14">
+        <f>H174/G174</f>
+        <v>1.4809781443720147E-4</v>
+      </c>
+      <c r="K174" s="19">
+        <f>J174</f>
+        <v>1.4809781443720147E-4</v>
+      </c>
+      <c r="L174" s="15">
+        <f>MIN(D174:D175)</f>
+        <v>7.9899170638030803</v>
+      </c>
+      <c r="M174" s="15">
+        <f>MAX(D174:D175)</f>
+        <v>7.9915906627761704</v>
+      </c>
+      <c r="N174" s="14">
+        <f>M174-L174</f>
+        <v>1.6735989730900513E-3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="14" t="s">
         <v>217</v>
       </c>
@@ -4650,7 +6103,7 @@
         <v>7.8658232744760301</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="14" t="s">
         <v>218</v>
       </c>
@@ -4663,8 +6116,40 @@
       <c r="E176" s="15">
         <v>7.7895329087663203</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G176" s="15">
+        <f>AVERAGE(D176:D177)</f>
+        <v>7.9177530067180655</v>
+      </c>
+      <c r="H176" s="14">
+        <f>_xlfn.STDEV.S(D176:D177)</f>
+        <v>1.0816194619316184E-3</v>
+      </c>
+      <c r="I176" s="14">
+        <f>2*H176</f>
+        <v>2.1632389238632368E-3</v>
+      </c>
+      <c r="J176" s="14">
+        <f>H176/G176</f>
+        <v>1.3660687078946319E-4</v>
+      </c>
+      <c r="K176" s="19">
+        <f>J176</f>
+        <v>1.3660687078946319E-4</v>
+      </c>
+      <c r="L176" s="15">
+        <f>MIN(D176:D177)</f>
+        <v>7.9169881862618698</v>
+      </c>
+      <c r="M176" s="15">
+        <f>MAX(D176:D177)</f>
+        <v>7.9185178271742602</v>
+      </c>
+      <c r="N176" s="14">
+        <f>M176-L176</f>
+        <v>1.5296409123903842E-3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="14" t="s">
         <v>219</v>
       </c>
@@ -4678,7 +6163,7 @@
         <v>7.7910625496787098</v>
       </c>
     </row>
-    <row r="178" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="14" t="s">
         <v>220</v>
       </c>
@@ -4691,8 +6176,40 @@
       <c r="E178" s="15">
         <v>7.7767419260336599</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G178" s="15">
+        <f>AVERAGE(D178:D179)</f>
+        <v>7.9164018860649001</v>
+      </c>
+      <c r="H178" s="14">
+        <f>_xlfn.STDEV.S(D178:D179)</f>
+        <v>4.4530902316816197E-6</v>
+      </c>
+      <c r="I178" s="14">
+        <f>2*H178</f>
+        <v>8.9061804633632394E-6</v>
+      </c>
+      <c r="J178" s="14">
+        <f>H178/G178</f>
+        <v>5.6251442205332128E-7</v>
+      </c>
+      <c r="K178" s="19">
+        <f>J178</f>
+        <v>5.6251442205332128E-7</v>
+      </c>
+      <c r="L178" s="15">
+        <f>MIN(D178:D179)</f>
+        <v>7.9163987372545996</v>
+      </c>
+      <c r="M178" s="15">
+        <f>MAX(D178:D179)</f>
+        <v>7.9164050348751998</v>
+      </c>
+      <c r="N178" s="14">
+        <f>M178-L178</f>
+        <v>6.2976206001152946E-6</v>
+      </c>
+    </row>
+    <row r="179" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="14" t="s">
         <v>221</v>
       </c>
@@ -4706,7 +6223,7 @@
         <v>7.77674822365426</v>
       </c>
     </row>
-    <row r="180" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="14" t="s">
         <v>222</v>
       </c>
@@ -4719,8 +6236,43 @@
       <c r="E180" s="15">
         <v>7.85323673583241</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F180" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="G180" s="15">
+        <f>AVERAGE(D180:D182)</f>
+        <v>7.9891642894530124</v>
+      </c>
+      <c r="H180" s="14">
+        <f>_xlfn.STDEV.S(D180:D182)</f>
+        <v>6.9723395988015496E-2</v>
+      </c>
+      <c r="I180" s="14">
+        <f>2*H180</f>
+        <v>0.13944679197603099</v>
+      </c>
+      <c r="J180" s="14">
+        <f>H180/G180</f>
+        <v>8.727245236408724E-3</v>
+      </c>
+      <c r="K180" s="19">
+        <f>J180</f>
+        <v>8.727245236408724E-3</v>
+      </c>
+      <c r="L180" s="15">
+        <f>MIN(D180:D181)</f>
+        <v>7.9253754091890798</v>
+      </c>
+      <c r="M180" s="15">
+        <f>MAX(D180:D181)</f>
+        <v>7.9785195004651799</v>
+      </c>
+      <c r="N180" s="14">
+        <f>M180-L180</f>
+        <v>5.3144091276100092E-2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="14" t="s">
         <v>223</v>
       </c>
@@ -4733,144 +6285,296 @@
       <c r="E181" s="15">
         <v>7.8000926445563001</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F181" s="16" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="182" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="B182" s="18">
+        <v>44130</v>
+      </c>
+      <c r="D182" s="15">
+        <v>8.0635979587047792</v>
+      </c>
+      <c r="E182" s="15">
+        <v>7.9383151940719996</v>
+      </c>
+      <c r="F182" s="16" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="183" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="B182" s="18">
+      <c r="B183" s="18">
         <v>44124</v>
       </c>
-      <c r="D182" s="15">
+      <c r="D183" s="15">
         <v>8.0525965489034004</v>
       </c>
-      <c r="E182" s="15">
+      <c r="E183" s="15">
         <v>7.86089245271185</v>
       </c>
     </row>
-    <row r="183" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="14" t="s">
+    <row r="184" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="14" t="s">
         <v>226</v>
-      </c>
-      <c r="B183" s="18">
-        <v>44130</v>
-      </c>
-      <c r="D183" s="15">
-        <v>8.0635979587047792</v>
-      </c>
-      <c r="E183" s="15">
-        <v>7.9383151940719996</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="14" t="s">
-        <v>227</v>
       </c>
       <c r="B184" s="18">
         <v>44130</v>
       </c>
       <c r="D184" s="15">
-        <v>7.9432763056151803</v>
+        <v>8.0635979587047792</v>
       </c>
       <c r="E184" s="15">
-        <v>7.8185701296753702</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7.9383151940719996</v>
+      </c>
+      <c r="G184" s="15"/>
+      <c r="K184" s="19"/>
+      <c r="L184" s="15"/>
+      <c r="M184" s="15"/>
+    </row>
+    <row r="185" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B185" s="18">
         <v>44130</v>
       </c>
       <c r="D185" s="15">
+        <v>7.9432763056151803</v>
+      </c>
+      <c r="E185" s="15">
+        <v>7.8185701296753702</v>
+      </c>
+      <c r="G185" s="15">
+        <f>AVERAGE(D185:D186)</f>
+        <v>7.9441268658156154</v>
+      </c>
+      <c r="H185" s="14">
+        <f>_xlfn.STDEV.S(D185:D186)</f>
+        <v>1.2028737710695655E-3</v>
+      </c>
+      <c r="I185" s="14">
+        <f>2*H185</f>
+        <v>2.4057475421391311E-3</v>
+      </c>
+      <c r="J185" s="14">
+        <f>H185/G185</f>
+        <v>1.5141673734411941E-4</v>
+      </c>
+      <c r="K185" s="19">
+        <f>J185</f>
+        <v>1.5141673734411941E-4</v>
+      </c>
+      <c r="L185" s="15">
+        <f>MIN(D185:D186)</f>
+        <v>7.9432763056151803</v>
+      </c>
+      <c r="M185" s="15">
+        <f>MAX(D185:D186)</f>
         <v>7.9449774260160497</v>
       </c>
-      <c r="E185" s="15">
-        <v>7.8202712500762397</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N185" s="14">
+        <f>M185-L185</f>
+        <v>1.7011204008694492E-3</v>
+      </c>
+    </row>
+    <row r="186" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B186" s="18">
         <v>44130</v>
       </c>
       <c r="D186" s="15">
-        <v>7.96372400233947</v>
+        <v>7.9449774260160497</v>
       </c>
       <c r="E186" s="15">
-        <v>7.84495774935416</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7.8202712500762397</v>
+      </c>
+    </row>
+    <row r="187" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B187" s="18">
         <v>44130</v>
       </c>
       <c r="D187" s="15">
+        <v>7.96372400233947</v>
+      </c>
+      <c r="E187" s="15">
+        <v>7.84495774935416</v>
+      </c>
+      <c r="G187" s="15">
+        <f>AVERAGE(D187:D188)</f>
+        <v>7.9782651410498353</v>
+      </c>
+      <c r="H187" s="14">
+        <f>_xlfn.STDEV.S(D187:D188)</f>
+        <v>2.0564275576546442E-2</v>
+      </c>
+      <c r="I187" s="14">
+        <f>2*H187</f>
+        <v>4.1128551153092885E-2</v>
+      </c>
+      <c r="J187" s="14">
+        <f>H187/G187</f>
+        <v>2.5775372481341794E-3</v>
+      </c>
+      <c r="K187" s="19">
+        <f>J187</f>
+        <v>2.5775372481341794E-3</v>
+      </c>
+      <c r="L187" s="15">
+        <f>MIN(D187:D188)</f>
+        <v>7.96372400233947</v>
+      </c>
+      <c r="M187" s="15">
+        <f>MAX(D187:D188)</f>
         <v>7.9928062797601998</v>
       </c>
-      <c r="E187" s="15">
-        <v>7.87404002677488</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N187" s="14">
+        <f>M187-L187</f>
+        <v>2.9082277420729774E-2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B188" s="18">
         <v>44130</v>
       </c>
       <c r="D188" s="15">
-        <v>8.0136910809783899</v>
+        <v>7.9928062797601998</v>
       </c>
       <c r="E188" s="15">
-        <v>7.87384793120167</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7.87404002677488</v>
+      </c>
+    </row>
+    <row r="189" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B189" s="18">
         <v>44130</v>
       </c>
       <c r="D189" s="15">
+        <v>8.0136910809783899</v>
+      </c>
+      <c r="E189" s="15">
+        <v>7.87384793120167</v>
+      </c>
+      <c r="G189" s="15">
+        <f>AVERAGE(D189:D190)</f>
+        <v>8.0003262029019897</v>
+      </c>
+      <c r="H189" s="14">
+        <f>_xlfn.STDEV.S(D189:D190)</f>
+        <v>1.8900791835107362E-2</v>
+      </c>
+      <c r="I189" s="14">
+        <f>2*H189</f>
+        <v>3.7801583670214724E-2</v>
+      </c>
+      <c r="J189" s="14">
+        <f>H189/G189</f>
+        <v>2.3625026474859744E-3</v>
+      </c>
+      <c r="K189" s="19">
+        <f>J189</f>
+        <v>2.3625026474859744E-3</v>
+      </c>
+      <c r="L189" s="15">
+        <f>MIN(D189:D190)</f>
         <v>7.9869613248255904</v>
       </c>
-      <c r="E189" s="15">
-        <v>7.8471181750488697</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M189" s="15">
+        <f>MAX(D189:D190)</f>
+        <v>8.0136910809783899</v>
+      </c>
+      <c r="N189" s="14">
+        <f>M189-L189</f>
+        <v>2.6729756152799489E-2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B190" s="18">
         <v>44130</v>
       </c>
       <c r="D190" s="15">
-        <v>7.8983132390663604</v>
+        <v>7.9869613248255904</v>
       </c>
       <c r="E190" s="15">
-        <v>7.7759694384276496</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7.8471181750488697</v>
+      </c>
+    </row>
+    <row r="191" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B191" s="18">
         <v>44130</v>
       </c>
       <c r="D191" s="15">
+        <v>7.8983132390663604</v>
+      </c>
+      <c r="E191" s="15">
+        <v>7.7759694384276496</v>
+      </c>
+      <c r="G191" s="15">
+        <f>AVERAGE(D191:D192)</f>
+        <v>7.9010076725656653</v>
+      </c>
+      <c r="H191" s="14">
+        <f>_xlfn.STDEV.S(D191:D192)</f>
+        <v>3.8105043976293463E-3</v>
+      </c>
+      <c r="I191" s="14">
+        <f>2*H191</f>
+        <v>7.6210087952586925E-3</v>
+      </c>
+      <c r="J191" s="14">
+        <f>H191/G191</f>
+        <v>4.8228081221340913E-4</v>
+      </c>
+      <c r="K191" s="19">
+        <f>J191</f>
+        <v>4.8228081221340913E-4</v>
+      </c>
+      <c r="L191" s="15">
+        <f>MIN(D191:D192)</f>
+        <v>7.8983132390663604</v>
+      </c>
+      <c r="M191" s="15">
+        <f>MAX(D191:D192)</f>
         <v>7.9037021060649701</v>
       </c>
-      <c r="E191" s="15">
+      <c r="N191" s="14">
+        <f>M191-L191</f>
+        <v>5.3888669986097426E-3</v>
+      </c>
+    </row>
+    <row r="192" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="B192" s="18">
+        <v>44130</v>
+      </c>
+      <c r="D192" s="15">
+        <v>7.9037021060649701</v>
+      </c>
+      <c r="E192" s="15">
         <v>7.7813583054262701</v>
       </c>
     </row>
@@ -4990,11 +6694,11 @@
         <v>8.1049089149999993</v>
       </c>
       <c r="C3" s="12">
-        <f t="shared" ref="C3:C64" si="0">$L$2</f>
+        <f t="shared" ref="C3:C10" si="0">$L$2</f>
         <v>8.0935490943465993</v>
       </c>
       <c r="D3" s="12">
-        <f t="shared" ref="D3:D64" si="1">B3-C3</f>
+        <f t="shared" ref="D3:D10" si="1">B3-C3</f>
         <v>1.1359820653400021E-2</v>
       </c>
       <c r="E3" s="13">
@@ -5118,7 +6822,7 @@
         <v>-1.2114369350999965E-2</v>
       </c>
       <c r="E7" s="13">
-        <f t="shared" ref="E7:E64" si="2">D7^2</f>
+        <f t="shared" ref="E7:E10" si="2">D7^2</f>
         <v>1.4675794477244731E-4</v>
       </c>
     </row>
@@ -5463,11 +7167,11 @@
         <v>7.8738051640000002</v>
       </c>
       <c r="D2" s="12">
-        <f t="shared" ref="D2:D25" si="0">B2-C2</f>
+        <f t="shared" ref="D2:D12" si="0">B2-C2</f>
         <v>0</v>
       </c>
       <c r="E2" s="13">
-        <f t="shared" ref="E2:E25" si="1">D2^2</f>
+        <f t="shared" ref="E2:E12" si="1">D2^2</f>
         <v>0</v>
       </c>
       <c r="F2" s="5"/>

</xml_diff>